<commit_message>
Skill Profile report created
</commit_message>
<xml_diff>
--- a/ocms/target/test-classes/TestData/SkillHistoricalReportData.xlsx
+++ b/ocms/target/test-classes/TestData/SkillHistoricalReportData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D7BA39-9669-4101-9D0C-4B5DB38D2E82}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -13,9 +14,8 @@
     <sheet name="ShowInNewPageDateRange" sheetId="5" r:id="rId4"/>
     <sheet name="ExportReport" sheetId="3" r:id="rId5"/>
     <sheet name="ExportReportDateRange" sheetId="6" r:id="rId6"/>
-    <sheet name="Queries" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="11">
   <si>
     <t>Report Channel</t>
   </si>
@@ -59,74 +59,11 @@
   <si>
     <t>OCM Skill Historical Report</t>
   </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>SELECT CONVERT(decimal(10,2), (100 * (sum(isnull(CallsHandledWithinSLAThreshold,0)))/
- (CAST(ISNULL((CASE WHEN SUM(isnull(PassedCalls,0))+sum(isnull(CallsAbandonedAfterSLAThreshold,0)) = 0 THEN 1
- else SUM(PassedCalls)+sum(isnull(CallsAbandonedAfterSLAThreshold,0)) end),1) AS float)))) AS [Service Level],
- SkillName as [Skill Name],sum([FlowIn]) AS [Flow In],sum([FlowOut]) AS [Flow Out],[SkillId] as [Skill ID],
- [dbo].[SECONDSTOhhmmss](sum(TotalStaffedTIme)/nullif(sum(TotalStaffedAgents),0)) AS [Avg Staff Time],
- [dbo].[SECONDSTOhhmmss](sum(TotalAbandTime)/nullif((sum(AbandCalls)+sum([AcdCalls])),0)) AS [Avg Aband Time],
- sum([AbandCalls]) AS [Aband Calls],
- [dbo].[SECONDSTOhhmmss](sum(SpeedOfAnswer)/nullif(sum([AcdCalls]),0)) AS [Avg Speed Answer],
- [dbo].[SECONDSTOhhmmss](sum([TotalAfterCallTime])) AS [Total After Call Time],
- [dbo].[SECONDSTOhhmmss](sum(TotalTalkTime)/nullif(sum([AcdCalls]),0)) AS [Avg Talk Time],
- sum([AcdCalls])  AS [Total Interaction],
- [dbo].[SECONDSTOhhmmss](sum(TotalAuxTime)) AS [Total Aux Time]
- from [OCM_SkillHistoricalReport]  WITH (NOLOCK)
- WHERE [ReportDateTime]&gt;='ReportBeforeDate' and [ReportDateTime]&lt;='ReportAfterDate' 
- GROUP BY [SkillId],[SkillName]
- ORDER BY [SkillName]</t>
-  </si>
-  <si>
-    <t>QueryDrillGridOne</t>
-  </si>
-  <si>
-    <t>SELECT CONVERT(decimal(10,2), (100 * (sum(isnull(CallsHandledWithinSLAThreshold,0)))/
-(CAST(ISNULL((CASE WHEN SUM(isnull(PassedCalls,0))+sum(isnull(CallsAbandonedAfterSLAThreshold,0)) = 0 THEN 1
-else SUM(PassedCalls)+sum(isnull(CallsAbandonedAfterSLAThreshold,0)) end),1) AS float))))  AS [Service Level],
-sum([FlowIn]) AS [Flow In],sum([FlowOut]) AS [Flow Out],
-[dbo].[SECONDSTOhhmmss](sum(TotalAbandTime)/nullif((sum(AbandCalls)+sum([AcdCalls])),0)) AS [Avg Aband Time],
-sum([AbandCalls]) AS [Aband Calls],
-Dateint AS [Date],[dbo].[SECONDSTOhhmmss](sum(SpeedOfAnswer)/nullif(sum([AcdCalls]),0)) AS [Avg Speed Answer], 
-[dbo].[SECONDSTOhhmmss](sum([TotalAfterCallTime])) AS [Total After Call Time],
-[dbo].[SECONDSTOhhmmss](sum(TotalTalkTime)/nullif(sum([AcdCalls]),0)) AS [Avg Talk Time],
-sum([AcdCalls]) AS [Total Interaction],
-[dbo].[SECONDSTOhhmmss](sum(TotalStaffedTIme)/nullif(sum(TotalStaffedAgents),0)) AS [Avg Staff],
-[dbo].[SECONDSTOhhmmss](sum(TotalAuxTime)) AS [Total Aux Time]
-from [OCM_SkillHistoricalReport] WITH (NOLOCK)
-WHERE [ReportDateTime]&gt;='ReportBeforeDate' and [ReportDateTime]&lt;='ReportAfterDate' and  SkillId like 'SkillIdCapturedFromUI'
-GROUP BY [Dateint],[SkillId],[SkillName] ORDER BY [Dateint] ASC</t>
-  </si>
-  <si>
-    <t>QueryDrillGridTwo</t>
-  </si>
-  <si>
-    <t>SELECT [ServiceLevel] AS [Service Level],[FlowIn] AS [Flow In],[FlowOut] AS [Flow Out],
-[dbo].[SECONDSTOhhmmss](TotalStaffedTIme/nullif(TotalStaffedAgents,0)) AS [Avg Staff Time],
-[dbo].[SECONDSTOhhmmss](TotalAbandTime/nullif((AbandCalls+[AcdCalls]),0)) AS [Avg Aband Time],
-[AbandCalls] AS [Aband Calls],
-[dbo].[SECONDSTOhhmmss](SpeedOfAnswer/nullif([AcdCalls],0)) AS [Avg Speed Answer],
-[dbo].[SECONDSTOhhmmss]([TotalAfterCallTime]) AS [Total After Call Time],
-[dbo].[SECONDSTOhhmmss](TotalTalkTime/nullif([AcdCalls],0)) AS [Avg Talk Time],
-[AcdCalls] AS [Total Interaction],[dbo].[SECONDSTOhhmmss](TotalAuxTime) AS [Total Aux Time],[Interval]
-FROM [OCM_SkillHistoricalReport] WITH (NOLOCK) WHERE [ReportDateTime]&gt;='ReportBeforeDate' AND [ReportDateTime]&lt;='ReportAfterDate' AND 
-[SkillId] like 'SkillIdCapturedFromUI' and [Interval] like '%' 
-ORDER BY [intvl] ASC</t>
-  </si>
-  <si>
-    <t>08-04-2020 00:00:00</t>
-  </si>
-  <si>
-    <t>22-04-2020 00:00:00</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,13 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,22 +375,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -492,22 +425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702A1EAB-F881-4B86-A3E3-081C46011C84}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -547,22 +480,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE176447-87D7-4EDC-896D-9D23F07DF512}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -596,22 +529,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60BEED6-9E0D-4C15-B8C6-0F6124EFA13A}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,7 +561,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -651,22 +584,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABD6B37-7362-47B2-8F62-99134BB2493A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -700,22 +633,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6DA6B1-CCD8-43EF-9A87-EEA417F7CC00}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -747,82 +680,6 @@
       </c>
       <c r="E2" t="s">
         <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>